<commit_message>
Add station number file
</commit_message>
<xml_diff>
--- a/Station-Numbers/Concat_Files_Suspect_Station_Numbers_20220910.xlsx
+++ b/Station-Numbers/Concat_Files_Suspect_Station_Numbers_20220910.xlsx
@@ -37,12 +37,375 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>ST-OUEN-VINCHELEZ-2.csv</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>[4432/4]</t>
+  </si>
+  <si>
+    <t>[4432/2]</t>
+  </si>
+  <si>
+    <t>ST-OUEN-VINCHELEZ.csv</t>
+  </si>
+  <si>
+    <t>ADLINGTON-STYPERSON-HOUSE.csv</t>
+  </si>
+  <si>
+    <t>Cheshire</t>
+  </si>
+  <si>
+    <t>[2728/2/9]</t>
+  </si>
+  <si>
+    <t>[2728/3/9]</t>
+  </si>
+  <si>
+    <t>[3!]</t>
+  </si>
+  <si>
+    <t>CHOLMONDELEY-SCHOOL-2.csv</t>
+  </si>
+  <si>
+    <t>[2962/3]</t>
+  </si>
+  <si>
+    <t>[2762/3]</t>
+  </si>
+  <si>
+    <t>CHOLMONDELEY-SCHOOL.csv</t>
+  </si>
+  <si>
+    <t>BUXTON-LIGHTWOOD-2.csv</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>Derbyshire</t>
+  </si>
+  <si>
+    <t>[2631]</t>
+  </si>
+  <si>
+    <t>[2681]</t>
+  </si>
+  <si>
+    <t>HAYFIELD-EDALE-CROSS-2.csv</t>
+  </si>
+  <si>
+    <t>[2643/4/5]</t>
+  </si>
+  <si>
+    <t>[2643/6/5]</t>
+  </si>
+  <si>
+    <t>HAYFIELD-TUNSTEAD-CLOUGH.csv</t>
+  </si>
+  <si>
+    <t>[2463/6/9]</t>
+  </si>
+  <si>
+    <t>[2643/6/9]</t>
+  </si>
+  <si>
+    <t>TAXAL-BLACKHILL-GATE-2.csv</t>
+  </si>
+  <si>
+    <t>[2643/6/1/3/4]</t>
+  </si>
+  <si>
+    <t>[2643/6/1/4]</t>
+  </si>
+  <si>
+    <t>EDMONDBYERS-FELDON-BURN.csv</t>
+  </si>
+  <si>
+    <t>Durham</t>
+  </si>
+  <si>
+    <t>[3553/3/2]</t>
+  </si>
+  <si>
+    <t>[3553/8/2]</t>
+  </si>
+  <si>
+    <t>ELLISFIELD-MANOR.csv</t>
+  </si>
+  <si>
+    <t>Hampshire</t>
+  </si>
+  <si>
+    <t>[628/9]</t>
+  </si>
+  <si>
+    <t>[728/9]</t>
+  </si>
+  <si>
+    <t>PENSHURST-SAINTS-HILL.csv</t>
+  </si>
+  <si>
+    <t>Kent-stayed-Kent</t>
+  </si>
+  <si>
+    <t>[335/3]</t>
+  </si>
+  <si>
+    <t>[335/5]</t>
+  </si>
+  <si>
+    <t>BOLTON-HEATON-RES-3.csv</t>
+  </si>
+  <si>
+    <t>Lancashire</t>
+  </si>
+  <si>
+    <t>[2047]</t>
+  </si>
+  <si>
+    <t>[2847]</t>
+  </si>
+  <si>
+    <t>HASLINGDEN-OGDEN-ONE.csv</t>
+  </si>
+  <si>
+    <t>[2919/30]</t>
+  </si>
+  <si>
+    <t>[2919/3]</t>
+  </si>
+  <si>
+    <t>CLEETHORPES-SIDNEY-PARK.csv</t>
+  </si>
+  <si>
+    <t>Lincolnshire</t>
+  </si>
+  <si>
+    <t>[2673/6]</t>
+  </si>
+  <si>
+    <t>[2573/6]</t>
+  </si>
+  <si>
+    <t>CAMPDEN-HILL-CAM-HOUSE-GARDENS.csv</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>Middlesex-became-London</t>
+  </si>
+  <si>
+    <t>[TQ249798]</t>
+  </si>
+  <si>
+    <t>[24]</t>
+  </si>
+  <si>
+    <t>WESTMINSTER-SPRING-GDNS-2.csv</t>
+  </si>
+  <si>
+    <t>[38/2]</t>
+  </si>
+  <si>
+    <t>[38]</t>
+  </si>
+  <si>
+    <t>[+]</t>
+  </si>
+  <si>
+    <t>WESTMINSTER-SPRING-GDNS.csv</t>
+  </si>
+  <si>
+    <t>[38/1]</t>
+  </si>
+  <si>
+    <t>ALPERTON-SEWAGE-WORKS.csv</t>
+  </si>
+  <si>
+    <t>Middlesex-stayed-Middlesex</t>
+  </si>
+  <si>
+    <t>[85]</t>
+  </si>
+  <si>
+    <t>[851]</t>
+  </si>
+  <si>
+    <t>BLANCHLAND-BIRKSIDE.csv</t>
+  </si>
+  <si>
+    <t>Northumberland</t>
+  </si>
+  <si>
+    <t>[3500/1/3]</t>
+  </si>
+  <si>
+    <t>[3560/1/3]</t>
+  </si>
+  <si>
+    <t>BLANCHLAND-COWBYERS.csv</t>
+  </si>
+  <si>
+    <t>[3500/1/4]</t>
+  </si>
+  <si>
+    <t>[3560/1/4]</t>
+  </si>
+  <si>
+    <t>FINNINGLEY-AIRFIELD.csv</t>
+  </si>
+  <si>
+    <t>Nottinghamshire</t>
+  </si>
+  <si>
+    <t>[0311/5/3]</t>
+  </si>
+  <si>
+    <t>[3111/5/3]</t>
+  </si>
+  <si>
+    <t>MANSFIELD-WW-RAINWORTH.csv</t>
+  </si>
+  <si>
+    <t>[26323]</t>
+  </si>
+  <si>
+    <t>[2623]</t>
+  </si>
+  <si>
+    <t>BISHOPS-CASTLE-THE-MOUNT-3.csv</t>
+  </si>
+  <si>
+    <t>Shropshire</t>
+  </si>
+  <si>
+    <t>[2274/2]</t>
+  </si>
+  <si>
+    <t>[2274]</t>
+  </si>
+  <si>
+    <t>BISHOPS-CASTLE-THE-MOUNT.csv</t>
+  </si>
+  <si>
+    <t>[2274/1]</t>
+  </si>
+  <si>
+    <t>CHURCH-STRETTON-WOOLSTASTON.csv</t>
+  </si>
+  <si>
+    <t>[2284/01]</t>
+  </si>
+  <si>
+    <t>[2284]</t>
+  </si>
+  <si>
+    <t>CRAVEN-ARMS-MIX-4.csv</t>
+  </si>
+  <si>
+    <t>[2273/20]</t>
+  </si>
+  <si>
+    <t>[2273/2]</t>
+  </si>
+  <si>
+    <t>OSWESTRY-LLANYBLODWEL.csv</t>
+  </si>
+  <si>
+    <t>[2310/12]</t>
+  </si>
+  <si>
+    <t>[2310/2]</t>
+  </si>
+  <si>
+    <t>ALCESTER-RAGLEY-2.csv</t>
+  </si>
+  <si>
+    <t>Warwickshire</t>
+  </si>
+  <si>
+    <t>[2447/1]</t>
+  </si>
+  <si>
+    <t>[2447]</t>
+  </si>
+  <si>
+    <t>APPLEBY-BONGATE-CROSS.csv</t>
+  </si>
+  <si>
+    <t>Westmorland</t>
+  </si>
+  <si>
+    <t>[3685/2]</t>
+  </si>
+  <si>
+    <t>[3685/1]</t>
+  </si>
+  <si>
+    <t>LEYBURN-BOLTON-HALL-2.csv</t>
+  </si>
+  <si>
+    <t>Yorkshire North Riding</t>
+  </si>
+  <si>
+    <t>[3423/01]</t>
+  </si>
+  <si>
+    <t>[3423]</t>
+  </si>
+  <si>
+    <t>BRADFORD-HEWENDEN-RES.csv</t>
+  </si>
+  <si>
+    <t>Yorkshire West Riding</t>
+  </si>
+  <si>
+    <t>[3276/01]</t>
+  </si>
+  <si>
+    <t>[3276]</t>
+  </si>
+  <si>
+    <t>EWDEN-VALLEY-MORE-HALL-RES-2.csv</t>
+  </si>
+  <si>
+    <t>[452688]</t>
+  </si>
+  <si>
+    <t>[3139/6]</t>
+  </si>
+  <si>
+    <t>KIRBY-MALZEARD-ARUNDO.csv</t>
+  </si>
+  <si>
+    <t>[3380/8]</t>
+  </si>
+  <si>
+    <t>[3380/5]</t>
+  </si>
+  <si>
+    <t>OLDHAM-STRINESDALE-2.csv</t>
+  </si>
+  <si>
+    <t>[435492]</t>
+  </si>
+  <si>
+    <t>[3092/5]</t>
+  </si>
+  <si>
+    <t>OLDHAM-STRINESDALE.csv</t>
+  </si>
+  <si>
     <t>CARRICKFERGUS-KNOCKAGH.csv</t>
   </si>
   <si>
-    <t>V2</t>
-  </si>
-  <si>
     <t>Antrim</t>
   </si>
   <si>
@@ -64,12 +427,57 @@
     <t>[5670/6]</t>
   </si>
   <si>
+    <t>HELENSBURGH-BLAIRNAIRN-2.csv</t>
+  </si>
+  <si>
+    <t>Dunbartonshire</t>
+  </si>
+  <si>
+    <t>[5326/1]</t>
+  </si>
+  <si>
+    <t>[5326/5]</t>
+  </si>
+  <si>
+    <t>HELENSBURGH-BLAIRNAIRN-3.csv</t>
+  </si>
+  <si>
+    <t>[5326/6]</t>
+  </si>
+  <si>
+    <t>HELENSBURGH-BLAIRNAIRN.csv</t>
+  </si>
+  <si>
+    <t>[5326/4]</t>
+  </si>
+  <si>
+    <t>EAGLESHAM-PICKETLAW-RES.csv</t>
+  </si>
+  <si>
+    <t>Renfrewshire</t>
+  </si>
+  <si>
+    <t>[5227/2]</t>
+  </si>
+  <si>
+    <t>[5277/2]</t>
+  </si>
+  <si>
+    <t>LOCH-FANNICH-THE-NEST-2.csv</t>
+  </si>
+  <si>
+    <t>Ross and Cromarty</t>
+  </si>
+  <si>
+    <t>[5773/7/1]</t>
+  </si>
+  <si>
+    <t>[5773/7]</t>
+  </si>
+  <si>
     <t>LAKE-COWLYD-CAPEL-CURIG-2.csv</t>
   </si>
   <si>
-    <t>V1</t>
-  </si>
-  <si>
     <t>Caernarfonshire</t>
   </si>
   <si>
@@ -79,9 +487,6 @@
     <t>[4346/5/1]</t>
   </si>
   <si>
-    <t>[3!]</t>
-  </si>
-  <si>
     <t>LAKE-COWLYD-CAPEL-CURIG.csv</t>
   </si>
   <si>
@@ -94,30 +499,6 @@
     <t>[4384/9]</t>
   </si>
   <si>
-    <t>ADLINGTON-STYPERSON-HOUSE.csv</t>
-  </si>
-  <si>
-    <t>Cheshire</t>
-  </si>
-  <si>
-    <t>[2728/2/9]</t>
-  </si>
-  <si>
-    <t>[2728/3/9]</t>
-  </si>
-  <si>
-    <t>CHOLMONDELEY-SCHOOL-2.csv</t>
-  </si>
-  <si>
-    <t>[2962/3]</t>
-  </si>
-  <si>
-    <t>[2762/3]</t>
-  </si>
-  <si>
-    <t>CHOLMONDELEY-SCHOOL.csv</t>
-  </si>
-  <si>
     <t>WREXHAM-WW-ERWAU-2.csv</t>
   </si>
   <si>
@@ -139,81 +520,6 @@
     <t>[4292/5]</t>
   </si>
   <si>
-    <t>BUXTON-LIGHTWOOD-2.csv</t>
-  </si>
-  <si>
-    <t>Derbyshire</t>
-  </si>
-  <si>
-    <t>[2631]</t>
-  </si>
-  <si>
-    <t>[2681]</t>
-  </si>
-  <si>
-    <t>HAYFIELD-EDALE-CROSS-2.csv</t>
-  </si>
-  <si>
-    <t>[2643/4/5]</t>
-  </si>
-  <si>
-    <t>[2643/6/5]</t>
-  </si>
-  <si>
-    <t>HAYFIELD-TUNSTEAD-CLOUGH.csv</t>
-  </si>
-  <si>
-    <t>[2463/6/9]</t>
-  </si>
-  <si>
-    <t>[2643/6/9]</t>
-  </si>
-  <si>
-    <t>TAXAL-BLACKHILL-GATE-2.csv</t>
-  </si>
-  <si>
-    <t>[2643/6/1/3/4]</t>
-  </si>
-  <si>
-    <t>[2643/6/1/4]</t>
-  </si>
-  <si>
-    <t>HELENSBURGH-BLAIRNAIRN-2.csv</t>
-  </si>
-  <si>
-    <t>Dunbartonshire</t>
-  </si>
-  <si>
-    <t>[5326/1]</t>
-  </si>
-  <si>
-    <t>[5326/5]</t>
-  </si>
-  <si>
-    <t>HELENSBURGH-BLAIRNAIRN-3.csv</t>
-  </si>
-  <si>
-    <t>[5326/6]</t>
-  </si>
-  <si>
-    <t>HELENSBURGH-BLAIRNAIRN.csv</t>
-  </si>
-  <si>
-    <t>[5326/4]</t>
-  </si>
-  <si>
-    <t>EDMONDBYERS-FELDON-BURN.csv</t>
-  </si>
-  <si>
-    <t>Durham</t>
-  </si>
-  <si>
-    <t>[3553/3/2]</t>
-  </si>
-  <si>
-    <t>[3553/8/2]</t>
-  </si>
-  <si>
     <t>BUCKLEY-HAWARDEN-WW.csv</t>
   </si>
   <si>
@@ -238,81 +544,6 @@
     <t>[4087]</t>
   </si>
   <si>
-    <t>[+]</t>
-  </si>
-  <si>
-    <t>ELLISFIELD-MANOR.csv</t>
-  </si>
-  <si>
-    <t>Hampshire</t>
-  </si>
-  <si>
-    <t>[628/9]</t>
-  </si>
-  <si>
-    <t>[728/9]</t>
-  </si>
-  <si>
-    <t>ST-OUEN-VINCHELEZ-2.csv</t>
-  </si>
-  <si>
-    <t>Jersey</t>
-  </si>
-  <si>
-    <t>[4432/4]</t>
-  </si>
-  <si>
-    <t>[4432/2]</t>
-  </si>
-  <si>
-    <t>ST-OUEN-VINCHELEZ.csv</t>
-  </si>
-  <si>
-    <t>PENSHURST-SAINTS-HILL.csv</t>
-  </si>
-  <si>
-    <t>Kent-stayed-Kent</t>
-  </si>
-  <si>
-    <t>[335/3]</t>
-  </si>
-  <si>
-    <t>[335/5]</t>
-  </si>
-  <si>
-    <t>BOLTON-HEATON-RES-3.csv</t>
-  </si>
-  <si>
-    <t>Lancashire</t>
-  </si>
-  <si>
-    <t>[2047]</t>
-  </si>
-  <si>
-    <t>[2847]</t>
-  </si>
-  <si>
-    <t>HASLINGDEN-OGDEN-ONE.csv</t>
-  </si>
-  <si>
-    <t>[2919/30]</t>
-  </si>
-  <si>
-    <t>[2919/3]</t>
-  </si>
-  <si>
-    <t>CLEETHORPES-SIDNEY-PARK.csv</t>
-  </si>
-  <si>
-    <t>Lincolnshire</t>
-  </si>
-  <si>
-    <t>[2673/6]</t>
-  </si>
-  <si>
-    <t>[2573/6]</t>
-  </si>
-  <si>
     <t>BALA-TEGID-STREET-2.csv</t>
   </si>
   <si>
@@ -346,48 +577,6 @@
     <t>[4330/5]</t>
   </si>
   <si>
-    <t>CAMPDEN-HILL-CAM-HOUSE-GARDENS.csv</t>
-  </si>
-  <si>
-    <t>V3</t>
-  </si>
-  <si>
-    <t>Middlesex-became-London</t>
-  </si>
-  <si>
-    <t>[TQ249798]</t>
-  </si>
-  <si>
-    <t>[24]</t>
-  </si>
-  <si>
-    <t>WESTMINSTER-SPRING-GDNS-2.csv</t>
-  </si>
-  <si>
-    <t>[38/2]</t>
-  </si>
-  <si>
-    <t>[38]</t>
-  </si>
-  <si>
-    <t>WESTMINSTER-SPRING-GDNS.csv</t>
-  </si>
-  <si>
-    <t>[38/1]</t>
-  </si>
-  <si>
-    <t>ALPERTON-SEWAGE-WORKS.csv</t>
-  </si>
-  <si>
-    <t>Middlesex-stayed-Middlesex</t>
-  </si>
-  <si>
-    <t>[85]</t>
-  </si>
-  <si>
-    <t>[851]</t>
-  </si>
-  <si>
     <t>LAKE-VYRNWY-HEN-GERRIG.csv</t>
   </si>
   <si>
@@ -418,48 +607,6 @@
     <t>[4268/5]</t>
   </si>
   <si>
-    <t>BLANCHLAND-BIRKSIDE.csv</t>
-  </si>
-  <si>
-    <t>Northumberland</t>
-  </si>
-  <si>
-    <t>[3500/1/3]</t>
-  </si>
-  <si>
-    <t>[3560/1/3]</t>
-  </si>
-  <si>
-    <t>BLANCHLAND-COWBYERS.csv</t>
-  </si>
-  <si>
-    <t>[3500/1/4]</t>
-  </si>
-  <si>
-    <t>[3560/1/4]</t>
-  </si>
-  <si>
-    <t>FINNINGLEY-AIRFIELD.csv</t>
-  </si>
-  <si>
-    <t>Nottinghamshire</t>
-  </si>
-  <si>
-    <t>[0311/5/3]</t>
-  </si>
-  <si>
-    <t>[3111/5/3]</t>
-  </si>
-  <si>
-    <t>MANSFIELD-WW-RAINWORTH.csv</t>
-  </si>
-  <si>
-    <t>[26323]</t>
-  </si>
-  <si>
-    <t>[2623]</t>
-  </si>
-  <si>
     <t>BIRMINGHAM-WW-FIGIN.csv</t>
   </si>
   <si>
@@ -470,153 +617,6 @@
   </si>
   <si>
     <t>[4242]</t>
-  </si>
-  <si>
-    <t>EAGLESHAM-PICKETLAW-RES.csv</t>
-  </si>
-  <si>
-    <t>Renfrewshire</t>
-  </si>
-  <si>
-    <t>[5227/2]</t>
-  </si>
-  <si>
-    <t>[5277/2]</t>
-  </si>
-  <si>
-    <t>LOCH-FANNICH-THE-NEST-2.csv</t>
-  </si>
-  <si>
-    <t>Ross and Cromarty</t>
-  </si>
-  <si>
-    <t>[5773/7/1]</t>
-  </si>
-  <si>
-    <t>[5773/7]</t>
-  </si>
-  <si>
-    <t>BISHOPS-CASTLE-THE-MOUNT-3.csv</t>
-  </si>
-  <si>
-    <t>Shropshire</t>
-  </si>
-  <si>
-    <t>[2274/2]</t>
-  </si>
-  <si>
-    <t>[2274]</t>
-  </si>
-  <si>
-    <t>BISHOPS-CASTLE-THE-MOUNT.csv</t>
-  </si>
-  <si>
-    <t>[2274/1]</t>
-  </si>
-  <si>
-    <t>CHURCH-STRETTON-WOOLSTASTON.csv</t>
-  </si>
-  <si>
-    <t>[2284/01]</t>
-  </si>
-  <si>
-    <t>[2284]</t>
-  </si>
-  <si>
-    <t>CRAVEN-ARMS-MIX-4.csv</t>
-  </si>
-  <si>
-    <t>[2273/20]</t>
-  </si>
-  <si>
-    <t>[2273/2]</t>
-  </si>
-  <si>
-    <t>OSWESTRY-LLANYBLODWEL.csv</t>
-  </si>
-  <si>
-    <t>[2310/12]</t>
-  </si>
-  <si>
-    <t>[2310/2]</t>
-  </si>
-  <si>
-    <t>ALCESTER-RAGLEY-2.csv</t>
-  </si>
-  <si>
-    <t>Warwickshire</t>
-  </si>
-  <si>
-    <t>[2447/1]</t>
-  </si>
-  <si>
-    <t>[2447]</t>
-  </si>
-  <si>
-    <t>APPLEBY-BONGATE-CROSS.csv</t>
-  </si>
-  <si>
-    <t>Westmorland</t>
-  </si>
-  <si>
-    <t>[3685/2]</t>
-  </si>
-  <si>
-    <t>[3685/1]</t>
-  </si>
-  <si>
-    <t>LEYBURN-BOLTON-HALL-2.csv</t>
-  </si>
-  <si>
-    <t>Yorkshire North Riding</t>
-  </si>
-  <si>
-    <t>[3423/01]</t>
-  </si>
-  <si>
-    <t>[3423]</t>
-  </si>
-  <si>
-    <t>BRADFORD-HEWENDEN-RES.csv</t>
-  </si>
-  <si>
-    <t>Yorkshire West Riding</t>
-  </si>
-  <si>
-    <t>[3276/01]</t>
-  </si>
-  <si>
-    <t>[3276]</t>
-  </si>
-  <si>
-    <t>EWDEN-VALLEY-MORE-HALL-RES-2.csv</t>
-  </si>
-  <si>
-    <t>[452688]</t>
-  </si>
-  <si>
-    <t>[3139/6]</t>
-  </si>
-  <si>
-    <t>KIRBY-MALZEARD-ARUNDO.csv</t>
-  </si>
-  <si>
-    <t>[3380/8]</t>
-  </si>
-  <si>
-    <t>[3380/5]</t>
-  </si>
-  <si>
-    <t>OLDHAM-STRINESDALE-2.csv</t>
-  </si>
-  <si>
-    <t>[435492]</t>
-  </si>
-  <si>
-    <t>[3092/5]</t>
-  </si>
-  <si>
-    <t>OLDHAM-STRINESDALE.csv</t>
   </si>
 </sst>
 </file>
@@ -1020,44 +1020,44 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>18</v>
@@ -1065,73 +1065,70 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
@@ -1139,79 +1136,79 @@
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>39</v>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1219,274 +1216,289 @@
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="F26" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>100</v>
@@ -1500,135 +1512,138 @@
         <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>125</v>
@@ -1639,96 +1654,87 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>20</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1736,144 +1742,141 @@
         <v>144</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="F46" s="1" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>169</v>
@@ -1887,161 +1890,158 @@
         <v>171</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>73</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>187</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>198</v>
+      <c r="F59" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>